<commit_message>
changes for admin, user dashboard
</commit_message>
<xml_diff>
--- a/Hospital_Management_System/src/test/resources/Sdet37TestData.xlsx
+++ b/Hospital_Management_System/src/test/resources/Sdet37TestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="User" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>TestID</t>
   </si>
@@ -238,6 +237,21 @@
   </si>
   <si>
     <t>Anuj</t>
+  </si>
+  <si>
+    <t>Sanjeev</t>
+  </si>
+  <si>
+    <t>Gayatri</t>
+  </si>
+  <si>
+    <t>2022-08-16 / 3:30 PM</t>
+  </si>
+  <si>
+    <t>Appointement Date/Time</t>
+  </si>
+  <si>
+    <t>Sarita Pandey</t>
   </si>
 </sst>
 </file>
@@ -576,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -584,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,9 +617,10 @@
     <col min="9" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,8 +654,11 @@
       <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -675,7 +693,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>33</v>
       </c>
@@ -699,6 +717,17 @@
       </c>
       <c r="J3" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -713,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +799,6 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
@@ -850,11 +878,17 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
       <c r="F6" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="7" t="s">
         <v>67</v>
       </c>
@@ -879,8 +913,6 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>

</xml_diff>